<commit_message>
Added asc excel files, updated setup and toml
</commit_message>
<xml_diff>
--- a/ccbhc_measurements/dashboard/excel files/DEP_REM_sub_1.xlsx
+++ b/ccbhc_measurements/dashboard/excel files/DEP_REM_sub_1.xlsx
@@ -3461,7 +3461,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4682,7 +4682,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -6827,7 +6827,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6926,7 +6926,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -13427,7 +13427,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -14879,7 +14879,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -18146,7 +18146,7 @@
       </c>
       <c r="E537" t="inlineStr">
         <is>
-          <t>Remission Period not Reached</t>
+          <t>No PHQ-9 Follow Up</t>
         </is>
       </c>
       <c r="F537" t="inlineStr">

</xml_diff>